<commit_message>
Finished time interval scripts
</commit_message>
<xml_diff>
--- a/docs/CABM site, instr, calibration, and config info.xlsx
+++ b/docs/CABM site, instr, calibration, and config info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31240" yWindow="1000" windowWidth="25600" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="3360" windowWidth="25600" windowHeight="14100" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="sites and dates" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Whistler" sheetId="4" r:id="rId7"/>
     <sheet name="checklist" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="96">
   <si>
     <t>East Trout Lake</t>
   </si>
@@ -249,12 +249,6 @@
     <t>(no data until 20150519)</t>
   </si>
   <si>
-    <t>distributions</t>
-  </si>
-  <si>
-    <t>fits</t>
-  </si>
-  <si>
     <t>ALERT</t>
   </si>
   <si>
@@ -319,6 +313,15 @@
   </si>
   <si>
     <t xml:space="preserve">power fall off in laser for #44 at Resolute </t>
+  </si>
+  <si>
+    <t>correction factors</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>xx/2</t>
   </si>
 </sst>
 </file>
@@ -742,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1539,7 +1542,7 @@
         <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>48</v>
@@ -1663,7 +1666,7 @@
         <v>42</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1673,7 +1676,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -1723,7 +1726,7 @@
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H22" s="7">
         <v>1</v>
@@ -1799,7 +1802,7 @@
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.15">
       <c r="D46" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1812,7 +1815,7 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4461,7 +4464,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="D4" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>50</v>
@@ -4545,13 +4548,13 @@
         <v>70</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>46</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>48</v>
@@ -4584,7 +4587,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C14" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>55</v>
@@ -4694,7 +4697,7 @@
         <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
@@ -4857,7 +4860,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -4874,8 +4877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4885,24 +4888,24 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
       </c>
       <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
         <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -4922,7 +4925,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -4942,7 +4945,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -4962,7 +4965,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -4982,7 +4985,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -5002,7 +5005,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
@@ -5022,17 +5025,47 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>94</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>87</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pulled down update to sp2_library
</commit_message>
<xml_diff>
--- a/docs/CABM site, instr, calibration, and config info.xlsx
+++ b/docs/CABM site, instr, calibration, and config info.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcallister/projects/CABM_sp2/docs/docs for ECCC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcallister/projects/CABM_sp2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="2760" windowWidth="25600" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="26260" yWindow="460" windowWidth="32100" windowHeight="15820" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Alert" sheetId="7" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Egbert" sheetId="3" r:id="rId3"/>
     <sheet name="Resolute" sheetId="6" r:id="rId4"/>
     <sheet name="Whistler" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="69">
   <si>
     <t>Whistler</t>
   </si>
@@ -178,6 +179,66 @@
   </si>
   <si>
     <t>NOTE: bytes per file changed to 1498 for this instr when installed at East Trout Lake</t>
+  </si>
+  <si>
+    <t>2009-2010</t>
+  </si>
+  <si>
+    <t>2013-2014</t>
+  </si>
+  <si>
+    <t>2015-2016</t>
+  </si>
+  <si>
+    <t>2014-2015</t>
+  </si>
+  <si>
+    <t>2011-2012</t>
+  </si>
+  <si>
+    <t>2012-2013</t>
+  </si>
+  <si>
+    <t>2013-2016</t>
+  </si>
+  <si>
+    <t>min VED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max VED </t>
+  </si>
+  <si>
+    <t>extrap?</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>HG calibs</t>
+  </si>
+  <si>
+    <t>LG calibs</t>
+  </si>
+  <si>
+    <t>rerun  ints</t>
+  </si>
+  <si>
+    <t>rerun distr corr</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>calib max</t>
+  </si>
+  <si>
+    <t>calib min</t>
+  </si>
+  <si>
+    <t>new min VED</t>
+  </si>
+  <si>
+    <t>new max VED</t>
   </si>
 </sst>
 </file>
@@ -247,7 +308,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -261,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -583,7 +647,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1091,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -3632,7 +3696,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4124,4 +4188,611 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="6" width="10.83203125" style="6"/>
+    <col min="7" max="7" width="13.33203125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="6" customWidth="1"/>
+    <col min="9" max="13" width="10.83203125" style="6"/>
+    <col min="14" max="14" width="15" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="6">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6">
+        <v>65</v>
+      </c>
+      <c r="E2" s="6">
+        <v>245</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="6">
+        <v>65</v>
+      </c>
+      <c r="H2" s="6">
+        <v>245</v>
+      </c>
+      <c r="I2" s="6">
+        <v>64</v>
+      </c>
+      <c r="J2" s="6">
+        <v>247</v>
+      </c>
+      <c r="K2" s="6">
+        <f>E2-J2</f>
+        <v>-2</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B3" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44</v>
+      </c>
+      <c r="D3" s="6">
+        <v>39</v>
+      </c>
+      <c r="E3" s="6">
+        <v>539</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="6">
+        <v>61</v>
+      </c>
+      <c r="J3" s="6">
+        <v>235</v>
+      </c>
+      <c r="K3" s="6">
+        <f>E3-J3</f>
+        <v>304</v>
+      </c>
+      <c r="L3" s="6">
+        <v>8</v>
+      </c>
+      <c r="M3" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="6">
+        <v>58</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45</v>
+      </c>
+      <c r="E4" s="6">
+        <v>555</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="6">
+        <v>74</v>
+      </c>
+      <c r="J4" s="6">
+        <v>441</v>
+      </c>
+      <c r="K4" s="6">
+        <f>E4-J4</f>
+        <v>114</v>
+      </c>
+      <c r="L4" s="6">
+        <v>12</v>
+      </c>
+      <c r="M4" s="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D5" s="6">
+        <v>64</v>
+      </c>
+      <c r="E5" s="6">
+        <v>854</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="6">
+        <v>74</v>
+      </c>
+      <c r="J5" s="6">
+        <v>338</v>
+      </c>
+      <c r="K5" s="6">
+        <f>E5-J5</f>
+        <v>516</v>
+      </c>
+      <c r="L5" s="6">
+        <v>14</v>
+      </c>
+      <c r="M5" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D6" s="6">
+        <v>71</v>
+      </c>
+      <c r="E6" s="6">
+        <v>891</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="6">
+        <v>80</v>
+      </c>
+      <c r="J6" s="6">
+        <v>336</v>
+      </c>
+      <c r="K6" s="6">
+        <f>E6-J6</f>
+        <v>555</v>
+      </c>
+      <c r="L6" s="6">
+        <v>16</v>
+      </c>
+      <c r="M6" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D7" s="6">
+        <v>80</v>
+      </c>
+      <c r="E7" s="6">
+        <v>830</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="6">
+        <v>85</v>
+      </c>
+      <c r="J7" s="6">
+        <v>337</v>
+      </c>
+      <c r="K7" s="6">
+        <f>E7-J7</f>
+        <v>493</v>
+      </c>
+      <c r="L7" s="6">
+        <v>18</v>
+      </c>
+      <c r="M7" s="6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D8" s="6">
+        <v>90</v>
+      </c>
+      <c r="E8" s="6">
+        <v>770</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="6">
+        <v>117</v>
+      </c>
+      <c r="J8" s="6">
+        <v>337</v>
+      </c>
+      <c r="K8" s="6">
+        <f>E8-J8</f>
+        <v>433</v>
+      </c>
+      <c r="L8" s="6">
+        <v>21</v>
+      </c>
+      <c r="M8" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="6">
+        <v>17</v>
+      </c>
+      <c r="D9" s="6">
+        <v>73</v>
+      </c>
+      <c r="E9" s="6">
+        <v>263</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="6">
+        <v>79</v>
+      </c>
+      <c r="J9" s="6">
+        <v>238</v>
+      </c>
+      <c r="K9" s="6">
+        <f>E9-J9</f>
+        <v>25</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6">
+        <v>58</v>
+      </c>
+      <c r="E10" s="6">
+        <v>238</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="6">
+        <v>66</v>
+      </c>
+      <c r="J10" s="6">
+        <v>213</v>
+      </c>
+      <c r="K10" s="6">
+        <f>E10-J10</f>
+        <v>25</v>
+      </c>
+      <c r="L10" s="6">
+        <v>6</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>85</v>
+      </c>
+      <c r="E11" s="6">
+        <v>245</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="6">
+        <v>85</v>
+      </c>
+      <c r="H11" s="6">
+        <v>245</v>
+      </c>
+      <c r="I11" s="6">
+        <v>86</v>
+      </c>
+      <c r="J11" s="6">
+        <v>235</v>
+      </c>
+      <c r="K11" s="6">
+        <f>E11-J11</f>
+        <v>10</v>
+      </c>
+      <c r="L11" s="6">
+        <v>23</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="6">
+        <v>17</v>
+      </c>
+      <c r="D12" s="6">
+        <v>61</v>
+      </c>
+      <c r="E12" s="6">
+        <v>251</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6">
+        <v>70</v>
+      </c>
+      <c r="H12" s="6">
+        <v>215</v>
+      </c>
+      <c r="I12" s="6">
+        <v>69</v>
+      </c>
+      <c r="J12" s="6">
+        <v>214</v>
+      </c>
+      <c r="K12" s="6">
+        <f>E12-J12</f>
+        <v>37</v>
+      </c>
+      <c r="L12" s="6">
+        <v>3</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D13" s="6">
+        <v>55</v>
+      </c>
+      <c r="E13" s="6">
+        <v>255</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6">
+        <v>65</v>
+      </c>
+      <c r="J13" s="6">
+        <v>235</v>
+      </c>
+      <c r="K13" s="6">
+        <f>E13-J13</f>
+        <v>20</v>
+      </c>
+      <c r="L13" s="6">
+        <v>4</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="D14" s="6">
+        <v>59</v>
+      </c>
+      <c r="E14" s="6">
+        <v>249</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="6">
+        <v>70</v>
+      </c>
+      <c r="J14" s="6">
+        <v>214</v>
+      </c>
+      <c r="K14" s="6">
+        <f>E14-J14</f>
+        <v>35</v>
+      </c>
+      <c r="L14" s="6">
+        <v>20</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="B15" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="6">
+        <v>44</v>
+      </c>
+      <c r="D15" s="6">
+        <v>64</v>
+      </c>
+      <c r="E15" s="6">
+        <v>714</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="6">
+        <v>72</v>
+      </c>
+      <c r="J15" s="6">
+        <v>369</v>
+      </c>
+      <c r="K15" s="6">
+        <f>E15-J15</f>
+        <v>345</v>
+      </c>
+      <c r="L15" s="6">
+        <v>11</v>
+      </c>
+      <c r="M15" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6">
+        <v>2009</v>
+      </c>
+      <c r="C16" s="6">
+        <v>17</v>
+      </c>
+      <c r="D16" s="6">
+        <v>85</v>
+      </c>
+      <c r="E16" s="6">
+        <v>245</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="6">
+        <v>85</v>
+      </c>
+      <c r="H16" s="6">
+        <v>245</v>
+      </c>
+      <c r="I16" s="6">
+        <v>86</v>
+      </c>
+      <c r="J16" s="6">
+        <v>235</v>
+      </c>
+      <c r="K16" s="6">
+        <f>E16-J16</f>
+        <v>10</v>
+      </c>
+      <c r="L16" s="6">
+        <v>23</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="B17" s="6">
+        <v>2010</v>
+      </c>
+      <c r="C17" s="6">
+        <v>17</v>
+      </c>
+      <c r="D17" s="6">
+        <v>65</v>
+      </c>
+      <c r="E17" s="6">
+        <v>245</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="6">
+        <v>65</v>
+      </c>
+      <c r="H17" s="6">
+        <v>245</v>
+      </c>
+      <c r="I17" s="6">
+        <v>64</v>
+      </c>
+      <c r="J17" s="6">
+        <v>247</v>
+      </c>
+      <c r="K17" s="6">
+        <f>E17-J17</f>
+        <v>-2</v>
+      </c>
+      <c r="L17" s="6">
+        <v>1</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>